<commit_message>
refactor: adding a simple method wich is removing the additional arbitrary line in the bottom
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,6 +1081,32 @@
         <v>1</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>100015</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BTBBIM03</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>100015</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>BTBBIM12</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1.234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>